<commit_message>
modificaciones de acceso y se agrego los diagramas de clase y de secuencia
</commit_message>
<xml_diff>
--- a/[Entrega 2] Sprint #1/Sprint backlog.xlsx
+++ b/[Entrega 2] Sprint #1/Sprint backlog.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="22">
   <si>
     <t>Sprint Backlog</t>
   </si>
@@ -33,7 +33,7 @@
     <t>Estado</t>
   </si>
   <si>
-    <t>0-01</t>
+    <t>0·01</t>
   </si>
   <si>
     <t>Entregable</t>
@@ -54,7 +54,7 @@
     <t>Agregar muestra de estadísticas posterior a la carga del residuo</t>
   </si>
   <si>
-    <t>0-04</t>
+    <t>0·04</t>
   </si>
   <si>
     <t>Crear lista general de productos reciclables</t>
@@ -63,6 +63,9 @@
     <t>Filtrado de productos según material</t>
   </si>
   <si>
+    <t>1·01</t>
+  </si>
+  <si>
     <t>Mostrar información principal (m3, veces que hubo recolección)</t>
   </si>
   <si>
@@ -70,6 +73,9 @@
   </si>
   <si>
     <t>Mapa virtual de geolocalización de los Puntos</t>
+  </si>
+  <si>
+    <t>2·01</t>
   </si>
   <si>
     <t>Diseño del informe principal sobre la recolección mensual</t>
@@ -295,14 +301,14 @@
       </c>
     </row>
     <row r="10" ht="15.75" customHeight="1">
-      <c r="A10" s="7">
-        <v>43466.0</v>
+      <c r="A10" s="5" t="s">
+        <v>15</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>8</v>
@@ -312,7 +318,7 @@
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
       <c r="C11" s="5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>8</v>
@@ -322,21 +328,21 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="13" ht="15.75" customHeight="1">
-      <c r="A13" s="7">
-        <v>43467.0</v>
+      <c r="A13" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>8</v>
@@ -346,7 +352,7 @@
       <c r="A14" s="7"/>
       <c r="B14" s="6"/>
       <c r="C14" s="5" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>8</v>

</xml_diff>